<commit_message>
Changes to schedule/Dorothea's sldies
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="940" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -108,9 +108,6 @@
     <t>Ben</t>
   </si>
   <si>
-    <t>Peter S?</t>
-  </si>
-  <si>
     <t>Linear factor models - Chapter 13</t>
   </si>
   <si>
@@ -132,14 +129,17 @@
     <t>(FIL summer party, so meet in morning)</t>
   </si>
   <si>
-    <t>Representation learning - Chapter 15</t>
+    <t>TensorFlow Session 2</t>
+  </si>
+  <si>
+    <t>Backpropogation (MATLAB tutorial)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -178,6 +178,28 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -196,7 +218,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="85">
+  <cellStyleXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -282,8 +304,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -296,8 +328,18 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="85">
+  <cellStyles count="95">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -340,6 +382,11 @@
     <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -382,6 +429,11 @@
     <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -716,10 +768,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="A1:D21"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -760,8 +812,8 @@
       <c r="A3" s="1">
         <v>42516</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>35</v>
+      <c r="B3" s="5" t="s">
+        <v>34</v>
       </c>
       <c r="C3" t="s">
         <v>17</v>
@@ -795,7 +847,7 @@
         <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -803,7 +855,13 @@
         <v>42537</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>27</v>
+        <v>36</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -814,7 +872,7 @@
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D7" t="s">
         <v>23</v>
@@ -824,7 +882,7 @@
       <c r="A8" s="1">
         <v>42551</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="9" t="s">
         <v>24</v>
       </c>
     </row>
@@ -832,52 +890,50 @@
       <c r="A9" s="1">
         <v>42558</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" t="s">
-        <v>25</v>
+      <c r="B9" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1">
         <v>42565</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" t="s">
-        <v>33</v>
+      <c r="B10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="1">
         <v>42572</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>27</v>
-      </c>
+      <c r="B11" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="7"/>
       <c r="E11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="1">
         <v>42579</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="B12" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="7" t="s">
         <v>22</v>
       </c>
     </row>
@@ -885,13 +941,13 @@
       <c r="A13" s="1">
         <v>42586</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="B13" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="7" t="s">
         <v>17</v>
       </c>
     </row>
@@ -899,79 +955,83 @@
       <c r="A14" s="1">
         <v>42593</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="8" t="s">
         <v>27</v>
       </c>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="1">
         <v>42600</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="B15" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D15" t="s">
-        <v>32</v>
+      <c r="D15" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="1">
         <v>42607</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="B16" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D16" t="s">
-        <v>29</v>
-      </c>
+      <c r="D16" s="7"/>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="1">
         <v>42614</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="8" t="s">
         <v>27</v>
       </c>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1">
         <v>42621</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="B18" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D18" t="s">
-        <v>33</v>
+      <c r="D18" s="7" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="1">
         <v>42628</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="9" t="s">
         <v>24</v>
       </c>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1">
         <v>42635</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="B20" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="7" t="s">
         <v>16</v>
       </c>
     </row>
@@ -979,15 +1039,39 @@
       <c r="A21" s="1">
         <v>42642</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="B21" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="7" t="s">
         <v>22</v>
       </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="7"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="7"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="7"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="7"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>